<commit_message>
Created utility for dashboard guest list validations Updated NA Data tables for Sept 2019 NA
</commit_message>
<xml_diff>
--- a/KatalonProjects/productData.xlsx
+++ b/KatalonProjects/productData.xlsx
@@ -2,28 +2,39 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\testautomation_new\NewArrivals\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\testautomation\KatalonProjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="249"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24975" windowHeight="10155"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$1</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Style</t>
   </si>
   <si>
+    <t>Description</t>
+  </si>
+  <si>
     <t>Color</t>
   </si>
   <si>
@@ -33,28 +44,28 @@
     <t>SzRange</t>
   </si>
   <si>
-    <t>Heather Gray</t>
+    <t>FinalContent</t>
+  </si>
+  <si>
+    <t>CareInstr</t>
   </si>
   <si>
     <t>XS-XL</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>FinalContent</t>
-  </si>
-  <si>
-    <t>CareInstr</t>
-  </si>
-  <si>
-    <t>Breeze Dress</t>
-  </si>
-  <si>
-    <t>96% Cotton, 4% Spandex</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;Turn garment inside out and place in a mesh bag. Machine wash separately in cold water on the delicate cycle. Only non-chlorine bleach if needed. Do not twist or wring. Lay flat to dry. Warm iron if needed. Can be dry cleaned.&lt;/div&gt;</t>
+    <t>3745</t>
+  </si>
+  <si>
+    <t>High Legging</t>
+  </si>
+  <si>
+    <t>Ganache</t>
+  </si>
+  <si>
+    <t>72% Rayon, 24% Nylon, 4% Spandex</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;Machine wash with like colors in cold water on the delicate cycle. Only non-chlorine bleach if needed. Lay flat to dry. Steam iron on the reverse side if needed. &lt;/div&gt;</t>
   </si>
 </sst>
 </file>
@@ -63,9 +74,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -114,7 +127,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
@@ -384,92 +397,7 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="1" cy="1"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst/>
-        </a:custGeom>
-        <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
-        </a:solidFill>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:round/>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:effectLst>
-                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="808080"/>
-                </a:outerShdw>
-              </a:effectLst>
-            </a14:hiddenEffects>
-          </a:ext>
-        </a:extLst>
-      </a:spPr>
-      <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" upright="1"/>
-      <a:lstStyle/>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="1" cy="1"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst/>
-        </a:custGeom>
-        <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
-        </a:solidFill>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:round/>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:effectLst>
-                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="808080"/>
-                </a:outerShdw>
-              </a:effectLst>
-            </a14:hiddenEffects>
-          </a:ext>
-        </a:extLst>
-      </a:spPr>
-      <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" upright="1"/>
-      <a:lstStyle/>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
@@ -484,73 +412,67 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="32.85546875" customWidth="1"/>
-    <col min="7" max="7" width="24.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>5618</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
+      <c r="C2" t="s">
+        <v>10</v>
       </c>
       <c r="D2" s="3">
-        <v>119</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>5</v>
+        <v>99</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter alignWithMargins="0">
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated createContactBO with changed locators for some of its elements
</commit_message>
<xml_diff>
--- a/KatalonProjects/productData.xlsx
+++ b/KatalonProjects/productData.xlsx
@@ -50,22 +50,22 @@
     <t>CareInstr</t>
   </si>
   <si>
-    <t>3841</t>
-  </si>
-  <si>
-    <t>Fringe Poncho</t>
-  </si>
-  <si>
-    <t>Poinsettia Red</t>
-  </si>
-  <si>
-    <t>XS/S-M/L</t>
-  </si>
-  <si>
-    <t>51% Cotton, 35% Viscose, 13% Nylon, 1% Spandex</t>
-  </si>
-  <si>
     <t>&lt;div&gt;Turn garment inside out and place in a mesh bag. Machine wash separately in cold water on the delicate cycle. Only non-chlorine bleach if needed. Do not twist or wring. Lay flat to dry. Warm iron if needed. Can be dry cleaned.&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>3842</t>
+  </si>
+  <si>
+    <t>Luxe Turtleneck</t>
+  </si>
+  <si>
+    <t>Winter White</t>
+  </si>
+  <si>
+    <t>XS-XL</t>
+  </si>
+  <si>
+    <t>51% Cotton, 30% Polyester, 19% Nylon</t>
   </si>
 </sst>
 </file>
@@ -451,25 +451,25 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3">
+        <v>99</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3">
-        <v>189</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NA script updated: PWL script updated for NA2
</commit_message>
<xml_diff>
--- a/KatalonProjects/productData.xlsx
+++ b/KatalonProjects/productData.xlsx
@@ -2,55 +2,140 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\testautomation\KatalonProjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24975" windowHeight="10155"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="249"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$1</definedName>
-  </definedNames>
   <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
   <si>
     <t>Style</t>
   </si>
   <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Retail</t>
+  </si>
+  <si>
+    <t>SzRange</t>
+  </si>
+  <si>
+    <t>XS-XL</t>
+  </si>
+  <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Color</t>
-  </si>
-  <si>
-    <t>Retail</t>
-  </si>
-  <si>
-    <t>SzRange</t>
-  </si>
-  <si>
     <t>FinalContent</t>
   </si>
   <si>
     <t>CareInstr</t>
   </si>
   <si>
-    <t>3846</t>
+    <t>&lt;div&gt;Turn garment inside out and place in a mesh bag. Machine wash separately in cold water on the delicate cycle. Only non-chlorine bleach if needed. Do not twist or wring. Lay flat to dry. Warm iron if needed. Can be dry cleaned.&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>M'Leggings</t>
+  </si>
+  <si>
+    <t>XS/S-M/L</t>
+  </si>
+  <si>
+    <t>Self: 100% Polyester Lining: 100% Polyester</t>
+  </si>
+  <si>
+    <t>100% Polyester</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;Wash by hand separately with cold water. Only non-chlorine bleach if needed. Do not twist or wring. Lay flat to dry. Steam iron only if needed. Can be dry cleaned. &lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;Machine wash with like colors in cold water on the delicate cycle. Only non-chlorine bleach if needed. Lay flat to dry. Warm iron if needed.&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;Turn garment inside out and place in a mesh bag. Machine wash separately in cold water on the delicate cycle. Only non-chlorine bleach if needed. Do not twist or wring. Lay flat to dry. Warm iron if needed. Can be washed by hand.&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>3875</t>
+  </si>
+  <si>
+    <t>Decked Out Dress</t>
+  </si>
+  <si>
+    <t>Twinkle Print</t>
+  </si>
+  <si>
+    <t>Self: 100% Polyester Belt Self: 100% Polyester Belt Lining: 100% Polyester</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;Turn garment inside out and place in a mesh bag. Machine wash separately in cold water on the delicate cycle. Only non-chlorine bleach if needed. Do not twist or wring. Lay flat to dry. Steam iron only if needed. Do not press with flat iron. Can be dry cleaned.&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>Cozy Cowl</t>
+  </si>
+  <si>
+    <t>Midnight and Black</t>
+  </si>
+  <si>
+    <t>96% Rayon, 4% Spandex</t>
+  </si>
+  <si>
+    <t>Fireside Hoodie</t>
+  </si>
+  <si>
+    <t>Deep Forest</t>
+  </si>
+  <si>
+    <t>3871</t>
+  </si>
+  <si>
+    <t>Snap Cowl</t>
+  </si>
+  <si>
+    <t>Storm</t>
+  </si>
+  <si>
+    <t>65% Modal, 32% Cotton, 3% Spandex</t>
+  </si>
+  <si>
+    <t>Snap Blouse</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;Machine wash separately, inside out, in cold water on the delicate cycle. Only non-chlorine bleach if needed. Lay flat to dry. Cool iron on the reverse side if needed. Can be dry cleaned.&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>Going Out Top</t>
+  </si>
+  <si>
+    <t>Party Plaid</t>
+  </si>
+  <si>
+    <t>Dressed-Up Shrug</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Self: 62% Cotton, 38% Acrylic Sleeve: 72% Acrylic, 28% Polyester Sleeve Lining: 100% Rayon</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;Turn garment inside out and place in a mesh bag. Machine wash separately in cold water on the delicate cycle. Only non-chlorine bleach if needed. Do not twist or wring. Lay flat to dry. Do not steam or iron faux fur.&lt;/div&gt;</t>
   </si>
   <si>
     <t>Windchill Wrap</t>
@@ -59,13 +144,37 @@
     <t>Winter Stripe</t>
   </si>
   <si>
-    <t>XS/S-M/L</t>
-  </si>
-  <si>
     <t>51% Cotton, 44% Acrylic, 5% Polyester</t>
   </si>
   <si>
     <t>&lt;div&gt;Dry clean for best results. Can be machine washed in a mesh bag in cold water on the delicate cycle. Only non-chlorine bleach. Lay flat to dry. Steam iron only if needed.&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>Victoria Blouse</t>
+  </si>
+  <si>
+    <t>Flourish Print</t>
+  </si>
+  <si>
+    <t>Purr Blouse</t>
+  </si>
+  <si>
+    <t>Emerald Skin Print</t>
+  </si>
+  <si>
+    <t>3850</t>
+  </si>
+  <si>
+    <t>Holiday Blazer</t>
+  </si>
+  <si>
+    <t>Holiday Plaid</t>
+  </si>
+  <si>
+    <t>96% Cotton, 4% Spandex</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;Turn garment inside out and place in a mesh bag. Machine wash separately in cold water, on the delicate cycle. Only non-chlorine bleach if needed. Do not twist or wring. Lay flat to dry. Warm iron if needed. Can be washed by hand.&lt;/div&gt;</t>
   </si>
 </sst>
 </file>
@@ -74,11 +183,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -123,17 +230,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
@@ -403,7 +507,92 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1" cy="1"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+        </a:solidFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:effectLst>
+                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="808080"/>
+                </a:outerShdw>
+              </a:effectLst>
+            </a14:hiddenEffects>
+          </a:ext>
+        </a:extLst>
+      </a:spPr>
+      <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" upright="1"/>
+      <a:lstStyle/>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1" cy="1"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+        </a:solidFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:effectLst>
+                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="808080"/>
+                </a:outerShdw>
+              </a:effectLst>
+            </a14:hiddenEffects>
+          </a:ext>
+        </a:extLst>
+      </a:spPr>
+      <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" upright="1"/>
+      <a:lstStyle/>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
@@ -415,70 +604,329 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1"/>
-    <col min="6" max="6" width="24.5703125" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="6" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="3">
+        <v>159</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>3869</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="3">
+        <v>94</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>3870</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="3">
+        <v>109</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="3">
+        <v>119</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>3857</v>
+      </c>
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="6">
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="3">
+        <v>84</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>3864</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="3">
+        <v>79</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>3865</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="3">
+        <v>89</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>3843</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="3">
+        <v>99</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>3846</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="3">
         <v>139</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E10" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="9" t="s">
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <v>3861</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="3">
+        <v>89</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
         <v>12</v>
       </c>
+      <c r="G11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>3863</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="3">
+        <v>84</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="3">
+        <v>169</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>